<commit_message>
Calculo fecha final producción
</commit_message>
<xml_diff>
--- a/planning/assets/formatsXlsx/Moldes.xlsx
+++ b/planning/assets/formatsXlsx/Moldes.xlsx
@@ -14,22 +14,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>tiempo_ensamblaje</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>molde</t>
   </si>
   <si>
     <t>referencia</t>
   </si>
+  <si>
+    <t>tiempo_montaje</t>
+  </si>
+  <si>
+    <t>tiempo_montaje_produccion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +65,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -71,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -144,6 +157,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -152,7 +187,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -178,6 +213,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -185,36 +232,7 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <strike val="0"/>
@@ -266,6 +284,30 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -297,17 +339,47 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="6" headerRowBorderDxfId="1" tableBorderDxfId="5">
-  <tableColumns count="3">
-    <tableColumn id="1" name="referencia" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <tableColumns count="4">
+    <tableColumn id="1" name="referencia" dataDxfId="3"/>
     <tableColumn id="2" name="molde" dataDxfId="2"/>
-    <tableColumn id="3" name="tiempo_ensamblaje" dataDxfId="3"/>
+    <tableColumn id="3" name="tiempo_montaje" dataDxfId="1"/>
+    <tableColumn id="4" name="tiempo_montaje_produccion" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -601,7 +673,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -609,7 +681,7 @@
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" customWidth="1"/>
@@ -627,44 +699,53 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18">
       <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>0</v>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="8"/>
       <c r="B2" s="5"/>
       <c r="C2" s="8"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="8"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="8"/>
       <c r="B5" s="5"/>
       <c r="C5" s="8"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="8"/>
       <c r="B6" s="5"/>
       <c r="C6" s="8"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="8"/>
       <c r="B7" s="6"/>
       <c r="C7" s="8"/>
+      <c r="D7" s="14"/>
     </row>
     <row r="13" spans="1:8">
       <c r="H13" s="4"/>

</xml_diff>